<commit_message>
Update with potential three new v2.5 resistors.
</commit_message>
<xml_diff>
--- a/kicad_files/D1 Mini - ESP8266 - Tubez/BOM/RatGDO-OpenSource-D1Mini-ESP8266-Tubez_BOM_JLCSMT.xlsx
+++ b/kicad_files/D1 Mini - ESP8266 - Tubez/BOM/RatGDO-OpenSource-D1Mini-ESP8266-Tubez_BOM_JLCSMT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\rat-ratgdo\kicad_files\D1 Mini - ESP8266\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\rat-ratgdo\kicad_files\D1 Mini - ESP8266 - Tubez\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD41584-BB27-4733-A14B-78A20444925D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AD4144-8C57-41ED-BD83-35C42A45A057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Comment</t>
   </si>
@@ -40,9 +40,6 @@
     <t>TerminalBlock_Phoenix_MKDS-1,5-3_1x03_P5.00mm_Horizontal</t>
   </si>
   <si>
-    <t>R3,R5,R4,R2,R1</t>
-  </si>
-  <si>
     <t>Q3,Q4,Q2</t>
   </si>
   <si>
@@ -94,83 +91,95 @@
     <t>C20917</t>
   </si>
   <si>
+    <t>C8545</t>
+  </si>
+  <si>
+    <t>C474904</t>
+  </si>
+  <si>
+    <t>C474905</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>B5819W</t>
+  </si>
+  <si>
+    <t>D_SOD-123</t>
+  </si>
+  <si>
+    <t>Converter_DCDC_RECOM_R-78HB-0.5_THT</t>
+  </si>
+  <si>
+    <t>K7805-500R3</t>
+  </si>
+  <si>
+    <t>C_0805_2012Metric_Pad1.18x1.45mm_HandSolder</t>
+  </si>
+  <si>
+    <t>10uF/50V</t>
+  </si>
+  <si>
+    <t>22uF/10V</t>
+  </si>
+  <si>
+    <t>SOT-23_Handsoldering</t>
+  </si>
+  <si>
+    <t>JLCPCB Part #（optional）</t>
+  </si>
+  <si>
+    <t>PinHeader_1x11_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Conn_01x11</t>
+  </si>
+  <si>
+    <t>C909662</t>
+  </si>
+  <si>
+    <t>C440198</t>
+  </si>
+  <si>
+    <t>C45783</t>
+  </si>
+  <si>
+    <t>R3,R5,R4,R2,R1,R6,R7</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>C17414</t>
+  </si>
+  <si>
+    <t>C17513</t>
+  </si>
+  <si>
+    <t>C8598</t>
+  </si>
+  <si>
     <t>C2128</t>
-  </si>
-  <si>
-    <t>C8545</t>
-  </si>
-  <si>
-    <t>C25612</t>
-  </si>
-  <si>
-    <t>C474904</t>
-  </si>
-  <si>
-    <t>C474905</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>B5819W</t>
-  </si>
-  <si>
-    <t>D_SOD-123</t>
-  </si>
-  <si>
-    <t>Converter_DCDC_RECOM_R-78HB-0.5_THT</t>
-  </si>
-  <si>
-    <t>K7805-500R3</t>
-  </si>
-  <si>
-    <t>C_0805_2012Metric_Pad1.18x1.45mm_HandSolder</t>
-  </si>
-  <si>
-    <t>10uF/50V</t>
-  </si>
-  <si>
-    <t>22uF/10V</t>
-  </si>
-  <si>
-    <t>SOT-23_Handsoldering</t>
-  </si>
-  <si>
-    <t>JLCPCB Part #（optional）</t>
-  </si>
-  <si>
-    <t>PinHeader_1x11_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>Conn_01x11</t>
-  </si>
-  <si>
-    <t>C64885</t>
-  </si>
-  <si>
-    <t>C909662</t>
-  </si>
-  <si>
-    <t>C440198</t>
-  </si>
-  <si>
-    <t>C45783</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -185,26 +194,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FFAFABAB"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -232,7 +221,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -243,27 +232,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -609,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="20" customHeight="1"/>
@@ -624,195 +592,209 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="20" customHeight="1">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="20" customHeight="1">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="20" customHeight="1">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" ht="20" customHeight="1">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
-      <c r="A6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" ht="20" customHeight="1">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" ht="20" customHeight="1">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
-      <c r="A7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
-      <c r="A8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="20" customHeight="1">
-      <c r="A9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="20" customHeight="1">
-      <c r="A10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" ht="20" customHeight="1">
-      <c r="A11" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" ht="20" customHeight="1">
-      <c r="A12" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" ht="20" customHeight="1">
-      <c r="A13" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="3"/>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Addition of R7/R6 and R8
</commit_message>
<xml_diff>
--- a/kicad_files/D1 Mini - ESP8266 - Tubez/BOM/RatGDO-OpenSource-D1Mini-ESP8266-Tubez_BOM_JLCSMT.xlsx
+++ b/kicad_files/D1 Mini - ESP8266 - Tubez/BOM/RatGDO-OpenSource-D1Mini-ESP8266-Tubez_BOM_JLCSMT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\rat-ratgdo\kicad_files\D1 Mini - ESP8266 - Tubez\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AD4144-8C57-41ED-BD83-35C42A45A057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8076A05E-99BD-474B-A140-9ACCD255D60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Comment</t>
   </si>
@@ -73,9 +73,6 @@
     <t>10k</t>
   </si>
   <si>
-    <t>WeMos_D1_mini</t>
-  </si>
-  <si>
     <t>J3</t>
   </si>
   <si>
@@ -142,9 +139,6 @@
     <t>PinHeader_1x11_P2.54mm_Vertical</t>
   </si>
   <si>
-    <t>Conn_01x11</t>
-  </si>
-  <si>
     <t>C909662</t>
   </si>
   <si>
@@ -173,6 +167,15 @@
   </si>
   <si>
     <t>C2128</t>
+  </si>
+  <si>
+    <t>DNP</t>
+  </si>
+  <si>
+    <t>Conn_01x11 - DNP</t>
+  </si>
+  <si>
+    <t>WeMos_D1_mini - DNP</t>
   </si>
 </sst>
 </file>
@@ -580,7 +583,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="20" customHeight="1"/>
@@ -602,13 +605,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -617,13 +620,13 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -631,7 +634,9 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3"/>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
@@ -639,13 +644,13 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E4" s="3"/>
     </row>
@@ -657,10 +662,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="3"/>
     </row>
@@ -675,7 +680,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -687,113 +692,115 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8"/>
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="20" customHeight="1">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" ht="20" customHeight="1">
       <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="20" customHeight="1">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="20" customHeight="1">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="20" customHeight="1">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" ht="20" customHeight="1">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 500mA fuse to input power
fuse is expensive on jlcpcb.  need to explore other part numbers., maybe move to 1206 size ptc instead.
</commit_message>
<xml_diff>
--- a/kicad_files/D1 Mini - ESP8266 - Tubez/BOM/RatGDO-OpenSource-D1Mini-ESP8266-Tubez_BOM_JLCSMT.xlsx
+++ b/kicad_files/D1 Mini - ESP8266 - Tubez/BOM/RatGDO-OpenSource-D1Mini-ESP8266-Tubez_BOM_JLCSMT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\rat-ratgdo\kicad_files\D1 Mini - ESP8266 - Tubez\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\rat-ratgdo\kicad_files\D1 Mini - ESP8266 - Tubez\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8076A05E-99BD-474B-A140-9ACCD255D60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBC8A4D-8465-41C6-BB31-784C399F97DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Comment</t>
   </si>
@@ -176,6 +176,18 @@
   </si>
   <si>
     <t>WeMos_D1_mini - DNP</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>500mA</t>
+  </si>
+  <si>
+    <t>Fuse_0805_2012Metric_Pad1.15x1.40mm_HandSolder</t>
+  </si>
+  <si>
+    <t>C2649565</t>
   </si>
 </sst>
 </file>
@@ -580,21 +592,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="20" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="26" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" customWidth="1"/>
-    <col min="3" max="3" width="36.08984375" customWidth="1"/>
-    <col min="4" max="4" width="24.453125" customWidth="1"/>
+    <col min="2" max="2" width="12.375" customWidth="1"/>
+    <col min="3" max="3" width="36.125" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20" customHeight="1">
+    <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -609,7 +621,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -624,7 +636,7 @@
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -639,7 +651,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -654,7 +666,7 @@
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -669,7 +681,7 @@
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -684,7 +696,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -699,7 +711,7 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -714,7 +726,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="20" customHeight="1">
+    <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -729,7 +741,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="20" customHeight="1">
+    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -744,7 +756,7 @@
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="20" customHeight="1">
+    <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -759,7 +771,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="20" customHeight="1">
+    <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -774,7 +786,7 @@
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="20" customHeight="1">
+    <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -789,7 +801,7 @@
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="20" customHeight="1">
+    <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -801,6 +813,20 @@
       </c>
       <c r="D14" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change to 750mA fuse 1206 package
</commit_message>
<xml_diff>
--- a/kicad_files/D1 Mini - ESP8266 - Tubez/BOM/RatGDO-OpenSource-D1Mini-ESP8266-Tubez_BOM_JLCSMT.xlsx
+++ b/kicad_files/D1 Mini - ESP8266 - Tubez/BOM/RatGDO-OpenSource-D1Mini-ESP8266-Tubez_BOM_JLCSMT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\rat-ratgdo\kicad_files\D1 Mini - ESP8266 - Tubez\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\rat-ratgdo\kicad_files\D1 Mini - ESP8266 - Tubez\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBC8A4D-8465-41C6-BB31-784C399F97DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3278B91D-5B3D-48E3-9D4F-356273BDAE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37730" yWindow="3740" windowWidth="28800" windowHeight="15450" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -181,13 +181,13 @@
     <t>F1</t>
   </si>
   <si>
-    <t>500mA</t>
-  </si>
-  <si>
-    <t>Fuse_0805_2012Metric_Pad1.15x1.40mm_HandSolder</t>
-  </si>
-  <si>
-    <t>C2649565</t>
+    <t>750mA</t>
+  </si>
+  <si>
+    <t>C328915</t>
+  </si>
+  <si>
+    <t>Fuse_1206_3216Metric_Pad1.42x1.75mm_HandSolder</t>
   </si>
 </sst>
 </file>
@@ -595,18 +595,18 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="20.149999999999999" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="26" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.375" customWidth="1"/>
-    <col min="3" max="3" width="36.125" customWidth="1"/>
-    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" customWidth="1"/>
+    <col min="3" max="3" width="36.08984375" customWidth="1"/>
+    <col min="4" max="4" width="24.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -621,7 +621,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="20.149999999999999" customHeight="1">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -636,7 +636,7 @@
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="20.149999999999999" customHeight="1">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -651,7 +651,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="20.149999999999999" customHeight="1">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -666,7 +666,7 @@
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="20.149999999999999" customHeight="1">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -681,7 +681,7 @@
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="20.149999999999999" customHeight="1">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -696,7 +696,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="20.149999999999999" customHeight="1">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -711,7 +711,7 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="20.149999999999999" customHeight="1">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -726,7 +726,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -741,7 +741,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="10" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -756,7 +756,7 @@
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -771,7 +771,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="12" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -786,7 +786,7 @@
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="13" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -801,7 +801,7 @@
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="14" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -815,7 +815,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="15" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>53</v>
       </c>
@@ -823,10 +823,10 @@
         <v>52</v>
       </c>
       <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
         <v>54</v>
-      </c>
-      <c r="D15" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>